<commit_message>
add font-awesome icons to beginning of tweets
</commit_message>
<xml_diff>
--- a/server/employees.xlsx
+++ b/server/employees.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="2016-06-01" sheetId="1" r:id="rId1"/>
@@ -949,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1437,7 +1437,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A6" sqref="A6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1571,14 +1571,17 @@
       <c r="C6" t="s">
         <v>26</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1686,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1821,14 +1824,17 @@
       <c r="C6" t="s">
         <v>26</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>